<commit_message>
changes to py files and added neural networking
</commit_message>
<xml_diff>
--- a/Resources/Model Tracker.xlsx
+++ b/Resources/Model Tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/smith/Desktop/GitHub Repos/Wine-Quality-Snobs/Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F70C25CF-A141-3F4C-985C-44A7517BC3B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03ED5395-011C-D14A-954E-F40BBEF71FAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13320" yWindow="2760" windowWidth="28040" windowHeight="17440" xr2:uid="{951ABD57-AA22-DF4F-B64E-CD7AECC104B9}"/>
+    <workbookView xWindow="15840" yWindow="2780" windowWidth="28040" windowHeight="17440" xr2:uid="{951ABD57-AA22-DF4F-B64E-CD7AECC104B9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="88">
   <si>
     <t>Model</t>
   </si>
@@ -238,13 +238,84 @@
   </si>
   <si>
     <t>0.79/0.64/0.7</t>
+  </si>
+  <si>
+    <t>Layer 1 Units</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Layer 2 </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>Units</t>
+    </r>
+  </si>
+  <si>
+    <t>Output Layer Activation</t>
+  </si>
+  <si>
+    <t>Trial Number</t>
+  </si>
+  <si>
+    <t>Accuracy</t>
+  </si>
+  <si>
+    <t>relu</t>
+  </si>
+  <si>
+    <t>sigmoid</t>
+  </si>
+  <si>
+    <t>Compile Crossentropy</t>
+  </si>
+  <si>
+    <t>Binary</t>
+  </si>
+  <si>
+    <t>softmax</t>
+  </si>
+  <si>
+    <t>Unionized Neural Model Trials (50 Epochs)</t>
+  </si>
+  <si>
+    <t>Loss</t>
+  </si>
+  <si>
+    <t>softmax 3units</t>
+  </si>
+  <si>
+    <t>Sparse Categorical</t>
+  </si>
+  <si>
+    <t>Epochs</t>
+  </si>
+  <si>
+    <t>Layer 3 Units</t>
+  </si>
+  <si>
+    <t>Activation 3</t>
+  </si>
+  <si>
+    <t>Activation 2</t>
+  </si>
+  <si>
+    <t>Activation 1</t>
+  </si>
+  <si>
+    <t>n/a</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -252,13 +323,51 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -273,12 +382,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -593,23 +708,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC4FB994-43F2-6F4D-932B-6A7EEBC915CF}">
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:L42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27:H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="12" customWidth="1"/>
     <col min="2" max="2" width="14.5" customWidth="1"/>
-    <col min="3" max="3" width="13" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" customWidth="1"/>
     <col min="4" max="4" width="16.1640625" customWidth="1"/>
     <col min="5" max="5" width="14.33203125" customWidth="1"/>
-    <col min="6" max="6" width="15.5" customWidth="1"/>
-    <col min="7" max="7" width="13.5" customWidth="1"/>
+    <col min="6" max="10" width="20.33203125" customWidth="1"/>
+    <col min="11" max="11" width="18.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -617,7 +733,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -636,11 +752,11 @@
       <c r="F2" t="s">
         <v>18</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -659,11 +775,11 @@
       <c r="F3" t="s">
         <v>11</v>
       </c>
-      <c r="G3" t="s">
+      <c r="I3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -682,11 +798,14 @@
       <c r="F4" s="1">
         <v>0.76</v>
       </c>
-      <c r="G4" s="1">
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1">
         <v>0.77</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J4" s="1"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -705,11 +824,11 @@
       <c r="F5" t="s">
         <v>19</v>
       </c>
-      <c r="G5" t="s">
+      <c r="I5" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -717,7 +836,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -736,11 +855,11 @@
       <c r="F8" t="s">
         <v>18</v>
       </c>
-      <c r="G8" t="s">
+      <c r="I8" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -759,11 +878,11 @@
       <c r="F9" t="s">
         <v>31</v>
       </c>
-      <c r="G9" t="s">
+      <c r="I9" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -782,11 +901,14 @@
       <c r="F10" s="1">
         <v>0.76</v>
       </c>
-      <c r="G10" s="1">
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1">
         <v>0.81</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J10" s="1"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -805,19 +927,19 @@
       <c r="F11" t="s">
         <v>32</v>
       </c>
-      <c r="G11" t="s">
+      <c r="I11" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="5" t="s">
         <v>1</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -836,11 +958,13 @@
       <c r="F14" t="s">
         <v>39</v>
       </c>
-      <c r="G14" t="s">
+      <c r="G14" s="3" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H14" s="3"/>
+      <c r="J14" s="7"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>5</v>
       </c>
@@ -859,11 +983,13 @@
       <c r="F15" t="s">
         <v>52</v>
       </c>
-      <c r="G15" t="s">
+      <c r="G15" s="3" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H15" s="3"/>
+      <c r="J15" s="7"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>6</v>
       </c>
@@ -882,11 +1008,13 @@
       <c r="F16">
         <v>0.66</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="3">
         <v>0.74</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H16" s="3"/>
+      <c r="J16" s="7"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>7</v>
       </c>
@@ -905,19 +1033,21 @@
       <c r="F17" t="s">
         <v>53</v>
       </c>
-      <c r="G17" t="s">
+      <c r="G17" s="3" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+      <c r="H17" s="3"/>
+      <c r="J17" s="7"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A20" s="6" t="s">
         <v>2</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>0</v>
       </c>
@@ -927,7 +1057,7 @@
       <c r="C21" t="s">
         <v>36</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="3" t="s">
         <v>37</v>
       </c>
       <c r="E21" t="s">
@@ -940,7 +1070,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>5</v>
       </c>
@@ -950,7 +1080,7 @@
       <c r="C22" t="s">
         <v>58</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="3" t="s">
         <v>60</v>
       </c>
       <c r="E22" t="s">
@@ -963,7 +1093,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>6</v>
       </c>
@@ -973,7 +1103,7 @@
       <c r="C23">
         <v>0.56999999999999995</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="3">
         <v>0.71</v>
       </c>
       <c r="E23">
@@ -986,7 +1116,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>7</v>
       </c>
@@ -996,7 +1126,7 @@
       <c r="C24" t="s">
         <v>59</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="3" t="s">
         <v>61</v>
       </c>
       <c r="E24" t="s">
@@ -1007,6 +1137,478 @@
       </c>
       <c r="G24" t="s">
         <v>67</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>71</v>
+      </c>
+      <c r="B27" t="s">
+        <v>68</v>
+      </c>
+      <c r="C27" t="s">
+        <v>86</v>
+      </c>
+      <c r="D27" t="s">
+        <v>69</v>
+      </c>
+      <c r="E27" t="s">
+        <v>85</v>
+      </c>
+      <c r="F27" t="s">
+        <v>83</v>
+      </c>
+      <c r="G27" t="s">
+        <v>84</v>
+      </c>
+      <c r="H27" t="s">
+        <v>70</v>
+      </c>
+      <c r="I27" t="s">
+        <v>72</v>
+      </c>
+      <c r="J27" t="s">
+        <v>79</v>
+      </c>
+      <c r="K27" t="s">
+        <v>75</v>
+      </c>
+      <c r="L27" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>1</v>
+      </c>
+      <c r="B28">
+        <v>124</v>
+      </c>
+      <c r="C28" t="s">
+        <v>73</v>
+      </c>
+      <c r="D28">
+        <v>64</v>
+      </c>
+      <c r="E28" t="s">
+        <v>73</v>
+      </c>
+      <c r="F28" t="s">
+        <v>87</v>
+      </c>
+      <c r="G28" t="s">
+        <v>87</v>
+      </c>
+      <c r="H28" t="s">
+        <v>74</v>
+      </c>
+      <c r="I28" s="4">
+        <v>0.54500000000000004</v>
+      </c>
+      <c r="J28" s="4"/>
+      <c r="K28" t="s">
+        <v>76</v>
+      </c>
+      <c r="L28">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>2</v>
+      </c>
+      <c r="B29">
+        <v>124</v>
+      </c>
+      <c r="C29" t="s">
+        <v>74</v>
+      </c>
+      <c r="D29">
+        <v>64</v>
+      </c>
+      <c r="E29" t="s">
+        <v>73</v>
+      </c>
+      <c r="F29" t="s">
+        <v>87</v>
+      </c>
+      <c r="G29" t="s">
+        <v>87</v>
+      </c>
+      <c r="H29" t="s">
+        <v>74</v>
+      </c>
+      <c r="I29">
+        <v>54</v>
+      </c>
+      <c r="K29" t="s">
+        <v>76</v>
+      </c>
+      <c r="L29">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>3</v>
+      </c>
+      <c r="B30">
+        <v>64</v>
+      </c>
+      <c r="C30" t="s">
+        <v>74</v>
+      </c>
+      <c r="D30">
+        <v>16</v>
+      </c>
+      <c r="E30" t="s">
+        <v>73</v>
+      </c>
+      <c r="F30" t="s">
+        <v>87</v>
+      </c>
+      <c r="G30" t="s">
+        <v>87</v>
+      </c>
+      <c r="H30" t="s">
+        <v>74</v>
+      </c>
+      <c r="I30">
+        <v>54.95</v>
+      </c>
+      <c r="K30" t="s">
+        <v>76</v>
+      </c>
+      <c r="L30">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>4</v>
+      </c>
+      <c r="B31">
+        <v>64</v>
+      </c>
+      <c r="C31" t="s">
+        <v>73</v>
+      </c>
+      <c r="D31">
+        <v>16</v>
+      </c>
+      <c r="E31" t="s">
+        <v>73</v>
+      </c>
+      <c r="F31" t="s">
+        <v>87</v>
+      </c>
+      <c r="G31" t="s">
+        <v>87</v>
+      </c>
+      <c r="H31" t="s">
+        <v>74</v>
+      </c>
+      <c r="I31">
+        <v>53.96</v>
+      </c>
+      <c r="K31" t="s">
+        <v>76</v>
+      </c>
+      <c r="L31">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>5</v>
+      </c>
+      <c r="B32">
+        <v>64</v>
+      </c>
+      <c r="C32" t="s">
+        <v>74</v>
+      </c>
+      <c r="D32">
+        <v>16</v>
+      </c>
+      <c r="E32" t="s">
+        <v>73</v>
+      </c>
+      <c r="F32" t="s">
+        <v>87</v>
+      </c>
+      <c r="G32" t="s">
+        <v>87</v>
+      </c>
+      <c r="H32" t="s">
+        <v>77</v>
+      </c>
+      <c r="I32">
+        <v>63.69</v>
+      </c>
+      <c r="J32">
+        <v>0.76</v>
+      </c>
+      <c r="K32" t="s">
+        <v>81</v>
+      </c>
+      <c r="L32">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>71</v>
+      </c>
+      <c r="B36" t="s">
+        <v>68</v>
+      </c>
+      <c r="C36" t="s">
+        <v>86</v>
+      </c>
+      <c r="D36" t="s">
+        <v>69</v>
+      </c>
+      <c r="E36" t="s">
+        <v>85</v>
+      </c>
+      <c r="F36" t="s">
+        <v>83</v>
+      </c>
+      <c r="G36" t="s">
+        <v>84</v>
+      </c>
+      <c r="H36" t="s">
+        <v>70</v>
+      </c>
+      <c r="I36" t="s">
+        <v>72</v>
+      </c>
+      <c r="J36" t="s">
+        <v>79</v>
+      </c>
+      <c r="K36" t="s">
+        <v>75</v>
+      </c>
+      <c r="L36" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>1</v>
+      </c>
+      <c r="B37">
+        <v>124</v>
+      </c>
+      <c r="C37" t="s">
+        <v>73</v>
+      </c>
+      <c r="D37">
+        <v>64</v>
+      </c>
+      <c r="E37" t="s">
+        <v>73</v>
+      </c>
+      <c r="F37" t="s">
+        <v>87</v>
+      </c>
+      <c r="G37" t="s">
+        <v>87</v>
+      </c>
+      <c r="H37" t="s">
+        <v>74</v>
+      </c>
+      <c r="I37">
+        <v>60.25</v>
+      </c>
+      <c r="J37">
+        <v>-8375.76</v>
+      </c>
+      <c r="K37" t="s">
+        <v>76</v>
+      </c>
+      <c r="L37">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>2</v>
+      </c>
+      <c r="B38">
+        <v>124</v>
+      </c>
+      <c r="C38" t="s">
+        <v>73</v>
+      </c>
+      <c r="D38">
+        <v>64</v>
+      </c>
+      <c r="E38" t="s">
+        <v>73</v>
+      </c>
+      <c r="F38" t="s">
+        <v>87</v>
+      </c>
+      <c r="G38" t="s">
+        <v>87</v>
+      </c>
+      <c r="H38" t="s">
+        <v>80</v>
+      </c>
+      <c r="I38">
+        <v>60.5</v>
+      </c>
+      <c r="J38">
+        <v>0.78900000000000003</v>
+      </c>
+      <c r="K38" t="s">
+        <v>81</v>
+      </c>
+      <c r="L38">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>3</v>
+      </c>
+      <c r="B39" s="8">
+        <v>64</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="D39" s="8">
+        <v>16</v>
+      </c>
+      <c r="E39" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="F39" t="s">
+        <v>87</v>
+      </c>
+      <c r="G39" t="s">
+        <v>87</v>
+      </c>
+      <c r="H39" t="s">
+        <v>80</v>
+      </c>
+      <c r="I39">
+        <v>63.5</v>
+      </c>
+      <c r="J39">
+        <v>0.73</v>
+      </c>
+      <c r="K39" t="s">
+        <v>81</v>
+      </c>
+      <c r="L39">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>4</v>
+      </c>
+      <c r="B40" s="8">
+        <v>64</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="D40" s="8">
+        <v>16</v>
+      </c>
+      <c r="E40" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="F40" t="s">
+        <v>87</v>
+      </c>
+      <c r="G40" t="s">
+        <v>87</v>
+      </c>
+      <c r="H40" t="s">
+        <v>80</v>
+      </c>
+      <c r="I40">
+        <v>62.5</v>
+      </c>
+      <c r="J40">
+        <v>0.75</v>
+      </c>
+      <c r="K40" t="s">
+        <v>81</v>
+      </c>
+      <c r="L40">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>5</v>
+      </c>
+      <c r="B41">
+        <v>16</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="D41">
+        <v>4</v>
+      </c>
+      <c r="E41" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="F41" t="s">
+        <v>87</v>
+      </c>
+      <c r="G41" t="s">
+        <v>87</v>
+      </c>
+      <c r="H41" t="s">
+        <v>80</v>
+      </c>
+      <c r="I41">
+        <v>65.239999999999995</v>
+      </c>
+      <c r="J41">
+        <v>0.74</v>
+      </c>
+      <c r="K41" t="s">
+        <v>81</v>
+      </c>
+      <c r="L41">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>6</v>
+      </c>
+      <c r="B42">
+        <v>16</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="D42">
+        <v>4</v>
+      </c>
+      <c r="E42" s="8" t="s">
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
more neural network testing
</commit_message>
<xml_diff>
--- a/Resources/Model Tracker.xlsx
+++ b/Resources/Model Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/smith/Desktop/GitHub Repos/Wine-Quality-Snobs/Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03ED5395-011C-D14A-954E-F40BBEF71FAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBD7EBC7-9C70-4249-B0E4-21722C18C840}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15840" yWindow="2780" windowWidth="28040" windowHeight="17440" xr2:uid="{951ABD57-AA22-DF4F-B64E-CD7AECC104B9}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="89">
   <si>
     <t>Model</t>
   </si>
@@ -270,6 +270,9 @@
   </si>
   <si>
     <t>sigmoid</t>
+  </si>
+  <si>
+    <t>Red Neural Model Trials (50 Epochs)</t>
   </si>
   <si>
     <t>Compile Crossentropy</t>
@@ -711,7 +714,7 @@
   <dimension ref="A1:L42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27:H32"/>
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -726,7 +729,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
       <c r="B1" t="s">
@@ -752,7 +755,7 @@
       <c r="F2" t="s">
         <v>18</v>
       </c>
-      <c r="I2" t="s">
+      <c r="G2" t="s">
         <v>30</v>
       </c>
     </row>
@@ -775,7 +778,7 @@
       <c r="F3" t="s">
         <v>11</v>
       </c>
-      <c r="I3" t="s">
+      <c r="G3" t="s">
         <v>20</v>
       </c>
     </row>
@@ -798,11 +801,10 @@
       <c r="F4" s="1">
         <v>0.76</v>
       </c>
-      <c r="G4" s="1"/>
+      <c r="G4" s="1">
+        <v>0.77</v>
+      </c>
       <c r="H4" s="1"/>
-      <c r="I4" s="1">
-        <v>0.77</v>
-      </c>
       <c r="J4" s="1"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
@@ -824,12 +826,12 @@
       <c r="F5" t="s">
         <v>19</v>
       </c>
-      <c r="I5" t="s">
+      <c r="G5" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="A7" s="6" t="s">
         <v>2</v>
       </c>
       <c r="B7" t="s">
@@ -855,7 +857,7 @@
       <c r="F8" t="s">
         <v>18</v>
       </c>
-      <c r="I8" t="s">
+      <c r="G8" t="s">
         <v>30</v>
       </c>
     </row>
@@ -878,7 +880,7 @@
       <c r="F9" t="s">
         <v>31</v>
       </c>
-      <c r="I9" t="s">
+      <c r="G9" t="s">
         <v>33</v>
       </c>
     </row>
@@ -901,11 +903,10 @@
       <c r="F10" s="1">
         <v>0.76</v>
       </c>
-      <c r="G10" s="1"/>
+      <c r="G10" s="1">
+        <v>0.81</v>
+      </c>
       <c r="H10" s="1"/>
-      <c r="I10" s="1">
-        <v>0.81</v>
-      </c>
       <c r="J10" s="1"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
@@ -927,7 +928,7 @@
       <c r="F11" t="s">
         <v>32</v>
       </c>
-      <c r="I11" t="s">
+      <c r="G11" t="s">
         <v>34</v>
       </c>
     </row>
@@ -961,7 +962,7 @@
       <c r="G14" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="H14" s="3"/>
+      <c r="H14" s="7"/>
       <c r="J14" s="7"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
@@ -986,7 +987,7 @@
       <c r="G15" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="H15" s="3"/>
+      <c r="H15" s="7"/>
       <c r="J15" s="7"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
@@ -1011,7 +1012,7 @@
       <c r="G16" s="3">
         <v>0.74</v>
       </c>
-      <c r="H16" s="3"/>
+      <c r="H16" s="7"/>
       <c r="J16" s="7"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
@@ -1036,7 +1037,7 @@
       <c r="G17" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="H17" s="3"/>
+      <c r="H17" s="7"/>
       <c r="J17" s="7"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
@@ -1141,7 +1142,7 @@
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
@@ -1152,19 +1153,19 @@
         <v>68</v>
       </c>
       <c r="C27" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D27" t="s">
         <v>69</v>
       </c>
       <c r="E27" t="s">
+        <v>86</v>
+      </c>
+      <c r="F27" t="s">
+        <v>84</v>
+      </c>
+      <c r="G27" t="s">
         <v>85</v>
-      </c>
-      <c r="F27" t="s">
-        <v>83</v>
-      </c>
-      <c r="G27" t="s">
-        <v>84</v>
       </c>
       <c r="H27" t="s">
         <v>70</v>
@@ -1173,13 +1174,13 @@
         <v>72</v>
       </c>
       <c r="J27" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="K27" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="L27" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.2">
@@ -1199,10 +1200,10 @@
         <v>73</v>
       </c>
       <c r="F28" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G28" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H28" t="s">
         <v>74</v>
@@ -1212,7 +1213,7 @@
       </c>
       <c r="J28" s="4"/>
       <c r="K28" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="L28">
         <v>50</v>
@@ -1235,10 +1236,10 @@
         <v>73</v>
       </c>
       <c r="F29" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G29" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H29" t="s">
         <v>74</v>
@@ -1247,7 +1248,7 @@
         <v>54</v>
       </c>
       <c r="K29" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="L29">
         <v>50</v>
@@ -1270,10 +1271,10 @@
         <v>73</v>
       </c>
       <c r="F30" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G30" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H30" t="s">
         <v>74</v>
@@ -1282,7 +1283,7 @@
         <v>54.95</v>
       </c>
       <c r="K30" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="L30">
         <v>50</v>
@@ -1305,10 +1306,10 @@
         <v>73</v>
       </c>
       <c r="F31" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G31" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H31" t="s">
         <v>74</v>
@@ -1317,7 +1318,7 @@
         <v>53.96</v>
       </c>
       <c r="K31" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="L31">
         <v>50</v>
@@ -1340,13 +1341,13 @@
         <v>73</v>
       </c>
       <c r="F32" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G32" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H32" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="I32">
         <v>63.69</v>
@@ -1355,7 +1356,7 @@
         <v>0.76</v>
       </c>
       <c r="K32" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="L32">
         <v>50</v>
@@ -1363,7 +1364,7 @@
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.2">
@@ -1374,19 +1375,19 @@
         <v>68</v>
       </c>
       <c r="C36" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D36" t="s">
         <v>69</v>
       </c>
       <c r="E36" t="s">
+        <v>86</v>
+      </c>
+      <c r="F36" t="s">
+        <v>84</v>
+      </c>
+      <c r="G36" t="s">
         <v>85</v>
-      </c>
-      <c r="F36" t="s">
-        <v>83</v>
-      </c>
-      <c r="G36" t="s">
-        <v>84</v>
       </c>
       <c r="H36" t="s">
         <v>70</v>
@@ -1395,13 +1396,13 @@
         <v>72</v>
       </c>
       <c r="J36" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="K36" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="L36" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.2">
@@ -1421,10 +1422,10 @@
         <v>73</v>
       </c>
       <c r="F37" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G37" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H37" t="s">
         <v>74</v>
@@ -1436,7 +1437,7 @@
         <v>-8375.76</v>
       </c>
       <c r="K37" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="L37">
         <v>50</v>
@@ -1459,13 +1460,13 @@
         <v>73</v>
       </c>
       <c r="F38" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G38" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H38" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I38">
         <v>60.5</v>
@@ -1474,7 +1475,7 @@
         <v>0.78900000000000003</v>
       </c>
       <c r="K38" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="L38">
         <v>50</v>
@@ -1497,13 +1498,13 @@
         <v>73</v>
       </c>
       <c r="F39" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G39" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H39" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I39">
         <v>63.5</v>
@@ -1512,7 +1513,7 @@
         <v>0.73</v>
       </c>
       <c r="K39" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="L39">
         <v>20</v>
@@ -1535,13 +1536,13 @@
         <v>73</v>
       </c>
       <c r="F40" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G40" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H40" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I40">
         <v>62.5</v>
@@ -1550,7 +1551,7 @@
         <v>0.75</v>
       </c>
       <c r="K40" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="L40">
         <v>50</v>
@@ -1573,13 +1574,13 @@
         <v>73</v>
       </c>
       <c r="F41" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G41" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H41" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I41">
         <v>65.239999999999995</v>
@@ -1588,7 +1589,7 @@
         <v>0.74</v>
       </c>
       <c r="K41" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="L41">
         <v>50</v>

</xml_diff>